<commit_message>
add import battle result from excel - 2
all task finish.
add players' ranking
outputl battle result record  as  insert sql
</commit_message>
<xml_diff>
--- a/doc/battle.xlsx
+++ b/doc/battle.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="28035" windowHeight="13005" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="28035" windowHeight="12975"/>
   </bookViews>
   <sheets>
     <sheet name="第一周" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2680" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2741" uniqueCount="459">
   <si>
     <t>场次名称</t>
   </si>
@@ -1362,6 +1362,46 @@
   </si>
   <si>
     <t>180121 LoveKiss vs Qiaoge 3</t>
+  </si>
+  <si>
+    <t>=PSER=Ap</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>=PSER=Mihu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>=PSER=SR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>=PSER=Eatos</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>=PSER=qiaogege</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>=PSER=SR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>=PSER=fengqin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>=PSER=Eatos</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>守雷者账号</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>=PSER=fengqin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1955,7 +1995,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1963,6 +2003,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2309,12 +2352,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M149"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -3070,9 +3116,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A22" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="A22" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="B22" t="s">
         <v>77</v>
@@ -3109,9 +3154,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A23" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="A23" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="B23" t="s">
         <v>77</v>
@@ -3239,9 +3283,8 @@
       <c r="E26" t="s">
         <v>27</v>
       </c>
-      <c r="F26" t="e">
-        <f>PSER=SR</f>
-        <v>#NAME?</v>
+      <c r="F26" s="3" t="s">
+        <v>454</v>
       </c>
       <c r="G26" t="s">
         <v>91</v>
@@ -3278,9 +3321,8 @@
       <c r="E27" t="s">
         <v>27</v>
       </c>
-      <c r="F27" t="e">
-        <f>PSER=SR</f>
-        <v>#NAME?</v>
+      <c r="F27" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="G27" t="s">
         <v>91</v>
@@ -3431,9 +3473,8 @@
       <c r="E31" t="s">
         <v>21</v>
       </c>
-      <c r="F31" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="F31" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="G31" t="s">
         <v>103</v>
@@ -3470,9 +3511,8 @@
       <c r="E32" t="s">
         <v>21</v>
       </c>
-      <c r="F32" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="F32" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="G32" t="s">
         <v>103</v>
@@ -4216,9 +4256,8 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A52" t="e">
-        <f>PSER=Mihu</f>
-        <v>#NAME?</v>
+      <c r="A52" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="B52" t="s">
         <v>143</v>
@@ -4366,9 +4405,8 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A56" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="A56" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="B56" t="s">
         <v>77</v>
@@ -4405,9 +4443,8 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A57" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="A57" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="B57" t="s">
         <v>77</v>
@@ -5280,9 +5317,8 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A80" t="e">
-        <f>PSER=SR</f>
-        <v>#NAME?</v>
+      <c r="A80" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="B80" t="s">
         <v>91</v>
@@ -5994,9 +6030,8 @@
       <c r="E99" t="s">
         <v>27</v>
       </c>
-      <c r="F99" t="e">
-        <f>PSER=Mihu</f>
-        <v>#NAME?</v>
+      <c r="F99" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="G99" t="s">
         <v>143</v>
@@ -6033,9 +6068,8 @@
       <c r="E100" t="s">
         <v>27</v>
       </c>
-      <c r="F100" t="e">
-        <f>PSER=Mihu</f>
-        <v>#NAME?</v>
+      <c r="F100" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="G100" t="s">
         <v>143</v>
@@ -6072,9 +6106,8 @@
       <c r="E101" t="s">
         <v>27</v>
       </c>
-      <c r="F101" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="F101" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="G101" t="s">
         <v>77</v>
@@ -6111,9 +6144,8 @@
       <c r="E102" t="s">
         <v>27</v>
       </c>
-      <c r="F102" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="F102" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="G102" t="s">
         <v>77</v>
@@ -6565,9 +6597,8 @@
       <c r="E114" t="s">
         <v>21</v>
       </c>
-      <c r="F114" t="e">
-        <f>PSER=Eatos</f>
-        <v>#NAME?</v>
+      <c r="F114" s="3" t="s">
+        <v>452</v>
       </c>
       <c r="G114" t="s">
         <v>232</v>
@@ -6604,9 +6635,8 @@
       <c r="E115" t="s">
         <v>27</v>
       </c>
-      <c r="F115" t="e">
-        <f>PSER=Eatos</f>
-        <v>#NAME?</v>
+      <c r="F115" s="3" t="s">
+        <v>452</v>
       </c>
       <c r="G115" t="s">
         <v>232</v>
@@ -6643,9 +6673,8 @@
       <c r="E116" t="s">
         <v>21</v>
       </c>
-      <c r="F116" t="e">
-        <f>PSER=Eatos</f>
-        <v>#NAME?</v>
+      <c r="F116" s="3" t="s">
+        <v>452</v>
       </c>
       <c r="G116" t="s">
         <v>232</v>
@@ -6962,9 +6991,8 @@
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A125" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="A125" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="B125" t="s">
         <v>245</v>
@@ -7001,9 +7029,8 @@
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A126" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="A126" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="B126" t="s">
         <v>245</v>
@@ -7245,9 +7272,8 @@
       <c r="E132" t="s">
         <v>21</v>
       </c>
-      <c r="F132" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="F132" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="G132" t="s">
         <v>245</v>
@@ -7284,9 +7310,8 @@
       <c r="E133" t="s">
         <v>21</v>
       </c>
-      <c r="F133" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="F133" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="G133" t="s">
         <v>245</v>
@@ -7574,9 +7599,8 @@
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A141" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="A141" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="B141" t="s">
         <v>77</v>
@@ -7613,9 +7637,8 @@
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A142" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="A142" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="B142" t="s">
         <v>77</v>
@@ -7681,9 +7704,8 @@
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A144" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="A144" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="B144" t="s">
         <v>245</v>
@@ -7720,9 +7742,8 @@
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A145" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="A145" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="B145" t="s">
         <v>245</v>
@@ -7850,9 +7871,8 @@
       <c r="E148" t="s">
         <v>21</v>
       </c>
-      <c r="F148" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="F148" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="G148" t="s">
         <v>245</v>
@@ -7889,9 +7909,8 @@
       <c r="E149" t="s">
         <v>21</v>
       </c>
-      <c r="F149" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="F149" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="G149" t="s">
         <v>245</v>
@@ -7915,6 +7934,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7922,14 +7942,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="O159" sqref="O159"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F163" sqref="F163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.75" customWidth="1"/>
     <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="21.625" customWidth="1"/>
     <col min="6" max="6" width="18.375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -7979,7 +8000,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>457</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -8191,9 +8212,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A9" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="A9" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="B9" t="s">
         <v>77</v>
@@ -8230,9 +8250,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A10" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="A10" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="B10" t="s">
         <v>77</v>
@@ -8436,9 +8455,8 @@
       <c r="E15" t="s">
         <v>21</v>
       </c>
-      <c r="F15" t="e">
-        <f>PSER=SR</f>
-        <v>#NAME?</v>
+      <c r="F15" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="G15" t="s">
         <v>91</v>
@@ -8475,9 +8493,8 @@
       <c r="E16" t="s">
         <v>21</v>
       </c>
-      <c r="F16" t="e">
-        <f>PSER=SR</f>
-        <v>#NAME?</v>
+      <c r="F16" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="G16" t="s">
         <v>91</v>
@@ -8894,9 +8911,8 @@
       <c r="E27" t="s">
         <v>27</v>
       </c>
-      <c r="F27" t="e">
-        <f>PSER=Mihu</f>
-        <v>#NAME?</v>
+      <c r="F27" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="G27" t="s">
         <v>143</v>
@@ -8933,9 +8949,8 @@
       <c r="E28" t="s">
         <v>27</v>
       </c>
-      <c r="F28" t="e">
-        <f>PSER=Mihu</f>
-        <v>#NAME?</v>
+      <c r="F28" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="G28" t="s">
         <v>143</v>
@@ -9071,9 +9086,8 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A32" t="e">
-        <f>PSER=Eatos</f>
-        <v>#NAME?</v>
+      <c r="A32" s="3" t="s">
+        <v>456</v>
       </c>
       <c r="B32" t="s">
         <v>232</v>
@@ -9110,9 +9124,8 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A33" t="e">
-        <f>PSER=Eatos</f>
-        <v>#NAME?</v>
+      <c r="A33" s="3" t="s">
+        <v>456</v>
       </c>
       <c r="B33" t="s">
         <v>232</v>
@@ -9316,9 +9329,8 @@
       <c r="E38" t="s">
         <v>21</v>
       </c>
-      <c r="F38" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="F38" s="3" t="s">
+        <v>458</v>
       </c>
       <c r="G38" t="s">
         <v>103</v>
@@ -9355,9 +9367,8 @@
       <c r="E39" t="s">
         <v>21</v>
       </c>
-      <c r="F39" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="F39" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="G39" t="s">
         <v>103</v>
@@ -10040,9 +10051,8 @@
       <c r="E57" t="s">
         <v>21</v>
       </c>
-      <c r="F57" t="e">
-        <f>PSER=Eatos</f>
-        <v>#NAME?</v>
+      <c r="F57" s="3" t="s">
+        <v>456</v>
       </c>
       <c r="G57" t="s">
         <v>232</v>
@@ -10079,9 +10089,8 @@
       <c r="E58" t="s">
         <v>21</v>
       </c>
-      <c r="F58" t="e">
-        <f>PSER=Eatos</f>
-        <v>#NAME?</v>
+      <c r="F58" s="3" t="s">
+        <v>456</v>
       </c>
       <c r="G58" t="s">
         <v>232</v>
@@ -10179,9 +10188,8 @@
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A61" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="A61" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="B61" t="s">
         <v>103</v>
@@ -10218,9 +10226,8 @@
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A62" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="A62" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="B62" t="s">
         <v>103</v>
@@ -10459,9 +10466,8 @@
       <c r="E68" t="s">
         <v>144</v>
       </c>
-      <c r="F68" t="e">
-        <f>PSER=Ap</f>
-        <v>#NAME?</v>
+      <c r="F68" s="3" t="s">
+        <v>449</v>
       </c>
       <c r="G68" t="s">
         <v>77</v>
@@ -10591,9 +10597,8 @@
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A72" t="e">
-        <f>PSER=SR</f>
-        <v>#NAME?</v>
+      <c r="A72" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="B72" t="s">
         <v>91</v>
@@ -10630,9 +10635,8 @@
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A73" t="e">
-        <f>PSER=SR</f>
-        <v>#NAME?</v>
+      <c r="A73" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="B73" t="s">
         <v>91</v>
@@ -10669,9 +10673,8 @@
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A74" t="e">
-        <f>PSER=SR</f>
-        <v>#NAME?</v>
+      <c r="A74" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="B74" t="s">
         <v>91</v>
@@ -11331,9 +11334,8 @@
       <c r="E91" t="s">
         <v>21</v>
       </c>
-      <c r="F91" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="F91" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="G91" t="s">
         <v>103</v>
@@ -11370,9 +11372,8 @@
       <c r="E92" t="s">
         <v>27</v>
       </c>
-      <c r="F92" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="F92" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="G92" t="s">
         <v>103</v>
@@ -11409,9 +11410,8 @@
       <c r="E93" t="s">
         <v>21</v>
       </c>
-      <c r="F93" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="F93" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="G93" t="s">
         <v>103</v>
@@ -12079,9 +12079,8 @@
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A111" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="A111" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="B111" t="s">
         <v>103</v>
@@ -12118,9 +12117,8 @@
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A112" t="e">
-        <f>PSER=fengqin</f>
-        <v>#NAME?</v>
+      <c r="A112" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="B112" t="s">
         <v>103</v>
@@ -12729,9 +12727,8 @@
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A129" t="e">
-        <f>PSER=Mihu</f>
-        <v>#NAME?</v>
+      <c r="A129" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="B129" t="s">
         <v>143</v>
@@ -12768,9 +12765,8 @@
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A130" t="e">
-        <f>PSER=Mihu</f>
-        <v>#NAME?</v>
+      <c r="A130" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="B130" t="s">
         <v>143</v>
@@ -12997,9 +12993,8 @@
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A136" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="A136" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="B136" t="s">
         <v>245</v>
@@ -13036,9 +13031,8 @@
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A137" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="A137" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="B137" t="s">
         <v>245</v>
@@ -13075,9 +13069,8 @@
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A138" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="A138" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="B138" t="s">
         <v>245</v>
@@ -13114,9 +13107,8 @@
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A139" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="A139" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="B139" t="s">
         <v>245</v>
@@ -13890,9 +13882,8 @@
       <c r="E159" t="s">
         <v>27</v>
       </c>
-      <c r="F159" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="F159" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="G159" t="s">
         <v>245</v>
@@ -13929,9 +13920,8 @@
       <c r="E160" t="s">
         <v>27</v>
       </c>
-      <c r="F160" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="F160" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="G160" t="s">
         <v>245</v>
@@ -13968,9 +13958,8 @@
       <c r="E161" t="s">
         <v>21</v>
       </c>
-      <c r="F161" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="F161" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="G161" t="s">
         <v>245</v>
@@ -14007,9 +13996,8 @@
       <c r="E162" t="s">
         <v>27</v>
       </c>
-      <c r="F162" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="F162" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="G162" t="s">
         <v>245</v>
@@ -14046,9 +14034,8 @@
       <c r="E163" t="s">
         <v>27</v>
       </c>
-      <c r="F163" t="e">
-        <f>PSER=qiaogege</f>
-        <v>#NAME?</v>
+      <c r="F163" s="3" t="s">
+        <v>453</v>
       </c>
       <c r="G163" t="s">
         <v>245</v>

</xml_diff>